<commit_message>
Update some figures, make flowchart
</commit_message>
<xml_diff>
--- a/figures+tables/Compare_OpenET-WIMAS_WRG_FitStats_Formatted.xlsx
+++ b/figures+tables/Compare_OpenET-WIMAS_WRG_FitStats_Formatted.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s947z036\WorkGits\SD-6_MapWaterConservation\figures+tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE53D918-01DF-4652-AF3C-1B59B37A2585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07ECA774-0644-4047-887B-21B743DAD5CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="copy raw data here" sheetId="1" r:id="rId1"/>
-    <sheet name="Formatted table" sheetId="3" r:id="rId2"/>
+    <sheet name="raw - all WRGs" sheetId="1" r:id="rId1"/>
+    <sheet name="formatted - all WRGs" sheetId="3" r:id="rId2"/>
+    <sheet name="raw - simple WRGs" sheetId="4" r:id="rId3"/>
+    <sheet name="formatted - simple WRGs" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
   <si>
     <t>Algorithm</t>
   </si>
@@ -396,7 +398,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -423,6 +425,9 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -857,7 +862,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174954FC-3560-46B8-875C-4291803A546D}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -889,19 +894,19 @@
         <v>10</v>
       </c>
       <c r="B2" s="3">
-        <f>'copy raw data here'!C2</f>
+        <f>'raw - all WRGs'!C2</f>
         <v>0.74349043733634101</v>
       </c>
       <c r="C2" s="4">
-        <f>'copy raw data here'!B2</f>
+        <f>'raw - all WRGs'!B2</f>
         <v>-29.4</v>
       </c>
       <c r="D2" s="4">
-        <f>'copy raw data here'!E2</f>
+        <f>'raw - all WRGs'!E2</f>
         <v>0.928692447243329</v>
       </c>
       <c r="E2" s="5">
-        <f>'copy raw data here'!D2</f>
+        <f>'raw - all WRGs'!D2</f>
         <v>0.60356346447113396</v>
       </c>
     </row>
@@ -910,19 +915,19 @@
         <v>11</v>
       </c>
       <c r="B3" s="17">
-        <f>'copy raw data here'!C3</f>
+        <f>'raw - all WRGs'!C3</f>
         <v>0.84472743864157596</v>
       </c>
       <c r="C3" s="18">
-        <f>'copy raw data here'!B3</f>
+        <f>'raw - all WRGs'!B3</f>
         <v>12.9</v>
       </c>
       <c r="D3" s="18">
-        <f>'copy raw data here'!E3</f>
+        <f>'raw - all WRGs'!E3</f>
         <v>1.3660493018355599</v>
       </c>
       <c r="E3" s="19">
-        <f>'copy raw data here'!D3</f>
+        <f>'raw - all WRGs'!D3</f>
         <v>0.62015451485279505</v>
       </c>
     </row>
@@ -931,19 +936,19 @@
         <v>12</v>
       </c>
       <c r="B4" s="6">
-        <f>'copy raw data here'!C4</f>
+        <f>'raw - all WRGs'!C4</f>
         <v>0.74635829171337797</v>
       </c>
       <c r="C4" s="7">
-        <f>'copy raw data here'!B4</f>
+        <f>'raw - all WRGs'!B4</f>
         <v>-13.9</v>
       </c>
       <c r="D4" s="7">
-        <f>'copy raw data here'!E4</f>
+        <f>'raw - all WRGs'!E4</f>
         <v>1.08033256844143</v>
       </c>
       <c r="E4" s="8">
-        <f>'copy raw data here'!D4</f>
+        <f>'raw - all WRGs'!D4</f>
         <v>0.6089281564347</v>
       </c>
     </row>
@@ -952,19 +957,19 @@
         <v>13</v>
       </c>
       <c r="B5" s="17">
-        <f>'copy raw data here'!C5</f>
+        <f>'raw - all WRGs'!C5</f>
         <v>0.92046421133088696</v>
       </c>
       <c r="C5" s="18">
-        <f>'copy raw data here'!B5</f>
+        <f>'raw - all WRGs'!B5</f>
         <v>-40.9</v>
       </c>
       <c r="D5" s="18">
-        <f>'copy raw data here'!E5</f>
+        <f>'raw - all WRGs'!E5</f>
         <v>0.80608254529997103</v>
       </c>
       <c r="E5" s="19">
-        <f>'copy raw data here'!D5</f>
+        <f>'raw - all WRGs'!D5</f>
         <v>0.46822645079120701</v>
       </c>
     </row>
@@ -973,19 +978,19 @@
         <v>14</v>
       </c>
       <c r="B6" s="6">
-        <f>'copy raw data here'!C6</f>
+        <f>'raw - all WRGs'!C6</f>
         <v>0.78455346348008304</v>
       </c>
       <c r="C6" s="7">
-        <f>'copy raw data here'!B6</f>
+        <f>'raw - all WRGs'!B6</f>
         <v>-24</v>
       </c>
       <c r="D6" s="7">
-        <f>'copy raw data here'!E6</f>
+        <f>'raw - all WRGs'!E6</f>
         <v>0.96342100094975203</v>
       </c>
       <c r="E6" s="8">
-        <f>'copy raw data here'!D6</f>
+        <f>'raw - all WRGs'!D6</f>
         <v>0.55925621500540501</v>
       </c>
     </row>
@@ -994,19 +999,19 @@
         <v>15</v>
       </c>
       <c r="B7" s="17">
-        <f>'copy raw data here'!C7</f>
+        <f>'raw - all WRGs'!C7</f>
         <v>0.87810338680559996</v>
       </c>
       <c r="C7" s="18">
-        <f>'copy raw data here'!B7</f>
+        <f>'raw - all WRGs'!B7</f>
         <v>42.7</v>
       </c>
       <c r="D7" s="18">
-        <f>'copy raw data here'!E7</f>
+        <f>'raw - all WRGs'!E7</f>
         <v>1.3908322153116499</v>
       </c>
       <c r="E7" s="19">
-        <f>'copy raw data here'!D7</f>
+        <f>'raw - all WRGs'!D7</f>
         <v>0.67054333105544495</v>
       </c>
     </row>
@@ -1015,20 +1020,355 @@
         <v>16</v>
       </c>
       <c r="B8" s="10">
-        <f>'copy raw data here'!C8</f>
+        <f>'raw - all WRGs'!C8</f>
         <v>0.73479916717468197</v>
       </c>
       <c r="C8" s="11">
-        <f>'copy raw data here'!B8</f>
+        <f>'raw - all WRGs'!B8</f>
         <v>-16.600000000000001</v>
       </c>
       <c r="D8" s="11">
-        <f>'copy raw data here'!E8</f>
+        <f>'raw - all WRGs'!E8</f>
         <v>1.05969561462669</v>
       </c>
       <c r="E8" s="12">
-        <f>'copy raw data here'!D8</f>
+        <f>'raw - all WRGs'!D8</f>
         <v>0.62411197467359902</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCA0513D-AC71-4EDB-BE75-88CB8788356C}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>-35.5</v>
+      </c>
+      <c r="C2">
+        <v>0.64236578016942403</v>
+      </c>
+      <c r="D2">
+        <v>0.27127328130709299</v>
+      </c>
+      <c r="E2">
+        <v>0.73073188677714296</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>3.9</v>
+      </c>
+      <c r="C3">
+        <v>0.64100551487593405</v>
+      </c>
+      <c r="D3">
+        <v>0.27375581649763697</v>
+      </c>
+      <c r="E3">
+        <v>0.99439206244612299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>-20.9</v>
+      </c>
+      <c r="C4">
+        <v>0.61820686485772802</v>
+      </c>
+      <c r="D4">
+        <v>0.27981023355653301</v>
+      </c>
+      <c r="E4">
+        <v>0.84696922688904497</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>-45.9</v>
+      </c>
+      <c r="C5">
+        <v>0.77320462929236899</v>
+      </c>
+      <c r="D5">
+        <v>0.209262556050543</v>
+      </c>
+      <c r="E5">
+        <v>0.67818615166065499</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>-31</v>
+      </c>
+      <c r="C6">
+        <v>0.66123445663315195</v>
+      </c>
+      <c r="D6">
+        <v>0.25439071056750601</v>
+      </c>
+      <c r="E6">
+        <v>0.76193852997043998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>33.9</v>
+      </c>
+      <c r="C7">
+        <v>0.63872081186159302</v>
+      </c>
+      <c r="D7">
+        <v>0.29571647620309</v>
+      </c>
+      <c r="E7">
+        <v>0.95811764316371195</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>-23.6</v>
+      </c>
+      <c r="C8">
+        <v>0.61178393848644297</v>
+      </c>
+      <c r="D8">
+        <v>0.29325253206296797</v>
+      </c>
+      <c r="E8">
+        <v>0.84286612540657502</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60528F09-3A8F-4106-BB3D-02BA64640A25}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3">
+        <f>'raw - simple WRGs'!C2</f>
+        <v>0.64236578016942403</v>
+      </c>
+      <c r="C2" s="4">
+        <f>'raw - simple WRGs'!B2</f>
+        <v>-35.5</v>
+      </c>
+      <c r="D2" s="4">
+        <f>'raw - simple WRGs'!E2</f>
+        <v>0.73073188677714296</v>
+      </c>
+      <c r="E2" s="5">
+        <f>'raw - simple WRGs'!D2</f>
+        <v>0.27127328130709299</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="21">
+        <f>'raw - simple WRGs'!C3</f>
+        <v>0.64100551487593405</v>
+      </c>
+      <c r="C3" s="22">
+        <f>'raw - simple WRGs'!B3</f>
+        <v>3.9</v>
+      </c>
+      <c r="D3" s="22">
+        <f>'raw - simple WRGs'!E3</f>
+        <v>0.99439206244612299</v>
+      </c>
+      <c r="E3" s="19">
+        <f>'raw - simple WRGs'!D3</f>
+        <v>0.27375581649763697</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="6">
+        <f>'raw - simple WRGs'!C4</f>
+        <v>0.61820686485772802</v>
+      </c>
+      <c r="C4" s="20">
+        <f>'raw - simple WRGs'!B4</f>
+        <v>-20.9</v>
+      </c>
+      <c r="D4" s="20">
+        <f>'raw - simple WRGs'!E4</f>
+        <v>0.84696922688904497</v>
+      </c>
+      <c r="E4" s="8">
+        <f>'raw - simple WRGs'!D4</f>
+        <v>0.27981023355653301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="21">
+        <f>'raw - simple WRGs'!C5</f>
+        <v>0.77320462929236899</v>
+      </c>
+      <c r="C5" s="22">
+        <f>'raw - simple WRGs'!B5</f>
+        <v>-45.9</v>
+      </c>
+      <c r="D5" s="22">
+        <f>'raw - simple WRGs'!E5</f>
+        <v>0.67818615166065499</v>
+      </c>
+      <c r="E5" s="19">
+        <f>'raw - simple WRGs'!D5</f>
+        <v>0.209262556050543</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="6">
+        <f>'raw - simple WRGs'!C6</f>
+        <v>0.66123445663315195</v>
+      </c>
+      <c r="C6" s="20">
+        <f>'raw - simple WRGs'!B6</f>
+        <v>-31</v>
+      </c>
+      <c r="D6" s="20">
+        <f>'raw - simple WRGs'!E6</f>
+        <v>0.76193852997043998</v>
+      </c>
+      <c r="E6" s="8">
+        <f>'raw - simple WRGs'!D6</f>
+        <v>0.25439071056750601</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="21">
+        <f>'raw - simple WRGs'!C7</f>
+        <v>0.63872081186159302</v>
+      </c>
+      <c r="C7" s="22">
+        <f>'raw - simple WRGs'!B7</f>
+        <v>33.9</v>
+      </c>
+      <c r="D7" s="22">
+        <f>'raw - simple WRGs'!E7</f>
+        <v>0.95811764316371195</v>
+      </c>
+      <c r="E7" s="19">
+        <f>'raw - simple WRGs'!D7</f>
+        <v>0.29571647620309</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="10">
+        <f>'raw - simple WRGs'!C8</f>
+        <v>0.61178393848644297</v>
+      </c>
+      <c r="C8" s="11">
+        <f>'raw - simple WRGs'!B8</f>
+        <v>-23.6</v>
+      </c>
+      <c r="D8" s="11">
+        <f>'raw - simple WRGs'!E8</f>
+        <v>0.84286612540657502</v>
+      </c>
+      <c r="E8" s="12">
+        <f>'raw - simple WRGs'!D8</f>
+        <v>0.29325253206296797</v>
       </c>
     </row>
   </sheetData>

</xml_diff>